<commit_message>
Changed FP Details Excel
</commit_message>
<xml_diff>
--- a/Reports/FP-Details.xlsx
+++ b/Reports/FP-Details.xlsx
@@ -1,19 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE39BBB4-951C-4E02-ABFA-3B9CCC67FD5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="67">
   <si>
     <t>CRUD Event</t>
   </si>
@@ -66,9 +62,6 @@
     <t>Name, Description, Date, Participants/Groups, Submit, Cancel</t>
   </si>
   <si>
-    <t>Create Event Request</t>
-  </si>
-  <si>
     <t>External Output</t>
   </si>
   <si>
@@ -87,49 +80,16 @@
     <t>Internal Logical Files</t>
   </si>
   <si>
-    <t>HTML, Controller, Confirm-HTML</t>
-  </si>
-  <si>
-    <t>id, name, description, date, participants/groups</t>
-  </si>
-  <si>
     <t xml:space="preserve">External Interface Files </t>
   </si>
   <si>
-    <t>Eventname, URL</t>
-  </si>
-  <si>
     <t>CRUD Group</t>
   </si>
   <si>
     <t>Name, Description, Public/Private, Participants, Icon, Submit, Cancel</t>
   </si>
   <si>
-    <t>Create Group Request</t>
-  </si>
-  <si>
-    <t>id, name, description, public/private, participants, icon</t>
-  </si>
-  <si>
-    <t>Groupname, URL</t>
-  </si>
-  <si>
     <t>Display Calendar</t>
-  </si>
-  <si>
-    <t>Month/Week/.., Calendar, Create-Event-Button, Display-Events</t>
-  </si>
-  <si>
-    <t>Journal</t>
-  </si>
-  <si>
-    <t>owner, content, date, events, month/week/…</t>
-  </si>
-  <si>
-    <t>Journal, User, Views</t>
-  </si>
-  <si>
-    <t>id, owner, content, date, events, month/week/…</t>
   </si>
   <si>
     <t>Register</t>
@@ -139,35 +99,10 @@
 </t>
   </si>
   <si>
-    <t>Name, Password</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Show Feed
-</t>
-  </si>
-  <si>
-    <t>Controller, Home-html, Feed-html</t>
-  </si>
-  <si>
-    <t>Username, Password, email, regDate, verifiied</t>
-  </si>
-  <si>
     <t>Edit What-to-bring List</t>
   </si>
   <si>
-    <t>OldPassword, NewPassword, repeat NewPassword</t>
-  </si>
-  <si>
-    <t>Modal</t>
-  </si>
-  <si>
     <t>Estimation:</t>
-  </si>
-  <si>
-    <t>Controller</t>
   </si>
   <si>
     <t xml:space="preserve">Low
@@ -180,36 +115,12 @@
     <t>Reply to Events</t>
   </si>
   <si>
-    <t>current password, old email, new email</t>
-  </si>
-  <si>
-    <t>Email to old address, Email to new address, Modal</t>
-  </si>
-  <si>
-    <t>Change Email HTML, Controller</t>
-  </si>
-  <si>
-    <t>emailUUID, username, creationdate, verified, Email-Template</t>
-  </si>
-  <si>
     <t>22.42</t>
   </si>
   <si>
-    <t>Email Interface</t>
-  </si>
-  <si>
     <t>Manage Subscriptions</t>
   </si>
   <si>
-    <t>Delete-btn, Confirmation Dialog</t>
-  </si>
-  <si>
-    <t>Modal, Email</t>
-  </si>
-  <si>
-    <t>deleteUUID, username, creationdate, Email-Template</t>
-  </si>
-  <si>
     <t>71.98</t>
   </si>
   <si>
@@ -226,12 +137,102 @@
   </si>
   <si>
     <t>Upcoming Use Cases</t>
+  </si>
+  <si>
+    <t>ID, Name, Description, Date, Participants/Groups</t>
+  </si>
+  <si>
+    <t>ID, Name, Description, Public/Private, Participants, Icon</t>
+  </si>
+  <si>
+    <t>Events, Groups, Users</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>Name, Description, Date, Participants/Groups</t>
+  </si>
+  <si>
+    <t>Name, Description, Public/Private, Participants, Icon</t>
+  </si>
+  <si>
+    <t>Groups, Users</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>View-Switch, Create-Event-Button</t>
+  </si>
+  <si>
+    <t>Display-Events</t>
+  </si>
+  <si>
+    <t>ID, User, Date, Event Time, Event Name, Location</t>
+  </si>
+  <si>
+    <t>Day, Week, Month, Next Events, Event Time, Event Name, Location</t>
+  </si>
+  <si>
+    <t>User, Events, Groups, Event-Replies</t>
+  </si>
+  <si>
+    <t>First Name, Last Name, E-Mail, Date of Birth, Location, Password, Submit</t>
+  </si>
+  <si>
+    <t>ID, Username, Password, E-Mail, Date of Birth, Location</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Accept, Reject, Details</t>
+  </si>
+  <si>
+    <t>Outstanding Responses</t>
+  </si>
+  <si>
+    <t>Event Name, Event Description</t>
+  </si>
+  <si>
+    <t>ID, Event Name, Event Description, Status</t>
+  </si>
+  <si>
+    <t>Events, Event-Replies</t>
+  </si>
+  <si>
+    <t>Events, Groups, Users, Event-Replies</t>
+  </si>
+  <si>
+    <t>Search Field, Search Button</t>
+  </si>
+  <si>
+    <t>Event Name/Group Name, Event Details/Groups Details</t>
+  </si>
+  <si>
+    <t>Event Name/Group Name, Event Details/Groups Details, Event Time</t>
+  </si>
+  <si>
+    <t>ID, Event Name/Group Name, Event Details/Groups Details, Event Time</t>
+  </si>
+  <si>
+    <t>Message Text, Submit</t>
+  </si>
+  <si>
+    <t>Message Text, Username, Time</t>
+  </si>
+  <si>
+    <t>ID, Username, Message Text, Time</t>
+  </si>
+  <si>
+    <t>Messages, Users, Events, Groups</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -451,10 +452,13 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,19 +471,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Tabellenblatt1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -744,14 +735,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
@@ -761,8 +752,8 @@
     <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="62" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="69.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
@@ -811,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G3" s="7">
         <v>12</v>
@@ -824,12 +815,12 @@
         <v>11</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>8</v>
@@ -841,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" s="7">
         <v>6</v>
@@ -851,7 +842,7 @@
         <v>10</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>10</v>
@@ -859,19 +850,19 @@
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G5" s="7">
         <v>6</v>
@@ -881,15 +872,15 @@
         <v>10</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="7">
         <v>3</v>
@@ -901,17 +892,17 @@
         <v>8</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="7">
         <v>0</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="8" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>10</v>
@@ -919,19 +910,19 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C7" s="13">
         <v>0</v>
       </c>
       <c r="D7" s="13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="13">
         <v>0</v>
@@ -941,7 +932,7 @@
         <v>10</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>10</v>
@@ -961,7 +952,7 @@
     </row>
     <row r="9" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1</v>
@@ -1005,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G10" s="7">
         <v>11</v>
@@ -1015,15 +1006,15 @@
         <v>10</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>8</v>
@@ -1035,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G11" s="7">
         <v>5</v>
@@ -1045,7 +1036,7 @@
         <v>10</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>10</v>
@@ -1053,19 +1044,19 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G12" s="7">
         <v>5</v>
@@ -1075,18 +1066,18 @@
         <v>10</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="7">
         <v>6</v>
@@ -1095,17 +1086,17 @@
         <v>8</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="7">
         <v>1</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="8" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="K13" s="10" t="s">
         <v>10</v>
@@ -1113,19 +1104,19 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14" s="13">
         <v>0</v>
       </c>
       <c r="D14" s="20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="13">
         <v>0</v>
@@ -1135,7 +1126,7 @@
         <v>10</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="K14" s="16" t="s">
         <v>10</v>
@@ -1155,7 +1146,7 @@
     </row>
     <row r="16" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>1</v>
@@ -1193,13 +1184,13 @@
         <v>8</v>
       </c>
       <c r="D17" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E17" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" s="7">
         <v>1</v>
@@ -1209,27 +1200,27 @@
         <v>10</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G18" s="7">
         <v>5</v>
@@ -1239,27 +1230,27 @@
         <v>10</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="7">
+        <v>7</v>
+      </c>
+      <c r="E19" s="7">
+        <v>4</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="7">
-        <v>5</v>
-      </c>
-      <c r="E19" s="7">
-        <v>1</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="G19" s="7">
         <v>0</v>
@@ -1269,18 +1260,18 @@
         <v>10</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="7">
         <v>6</v>
@@ -1289,17 +1280,17 @@
         <v>8</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" s="7">
         <v>0</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="8" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="K20" s="10" t="s">
         <v>10</v>
@@ -1307,7 +1298,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C21" s="13">
         <v>0</v>
@@ -1319,7 +1310,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" s="13">
         <v>0</v>
@@ -1349,7 +1340,7 @@
     </row>
     <row r="23" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>1</v>
@@ -1387,43 +1378,43 @@
         <v>8</v>
       </c>
       <c r="D24" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E24" s="7">
         <v>1</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" s="7">
         <v>8</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="8" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E25" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25" s="7">
         <v>1</v>
@@ -1432,16 +1423,16 @@
       <c r="I25" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J25" s="9" t="s">
-        <v>38</v>
+      <c r="J25" s="35" t="s">
+        <v>14</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>8</v>
@@ -1453,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G26" s="7">
         <v>1</v>
@@ -1471,29 +1462,29 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G27" s="7">
         <v>0</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="8" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="K27" s="10" t="s">
         <v>10</v>
@@ -1501,7 +1492,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C28" s="13">
         <v>0</v>
@@ -1513,7 +1504,7 @@
         <v>8</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G28" s="13">
         <v>0</v>
@@ -1555,7 +1546,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="30" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31"/>
@@ -1581,7 +1572,7 @@
     </row>
     <row r="33" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>1</v>
@@ -1625,25 +1616,19 @@
         <v>1</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G34" s="7">
         <v>4</v>
       </c>
       <c r="H34" s="7"/>
-      <c r="I34" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K34" s="23" t="s">
-        <v>37</v>
-      </c>
+      <c r="I34" s="8"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="23"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>8</v>
@@ -1661,49 +1646,37 @@
         <v>3</v>
       </c>
       <c r="H35" s="7"/>
-      <c r="I35" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="K35" s="23" t="s">
-        <v>10</v>
-      </c>
+      <c r="I35" s="8"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="23"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0</v>
+      </c>
+      <c r="F36" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="7">
-        <v>0</v>
-      </c>
-      <c r="E36" s="7">
-        <v>0</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="G36" s="7">
         <v>3</v>
       </c>
       <c r="H36" s="7"/>
-      <c r="I36" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J36" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="K36" s="23" t="s">
-        <v>10</v>
-      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="23"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C37" s="7">
         <v>1</v>
@@ -1715,27 +1688,21 @@
         <v>8</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G37" s="7">
         <v>0</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K37" s="10" t="s">
-        <v>10</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I37" s="8"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="10"/>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C38" s="13">
         <v>0</v>
@@ -1747,23 +1714,17 @@
         <v>8</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="G38" s="13">
         <v>0</v>
       </c>
       <c r="H38" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J38" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K38" s="16" t="s">
-        <v>10</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="I38" s="14"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="16"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" s="17"/>
@@ -1779,7 +1740,7 @@
     </row>
     <row r="40" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>1</v>
@@ -1820,10 +1781,10 @@
         <v>3</v>
       </c>
       <c r="E41" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G41" s="7">
         <v>5</v>
@@ -1833,27 +1794,27 @@
         <v>10</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K41" s="23" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E42" s="7">
         <v>0</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G42" s="7">
         <v>1</v>
@@ -1863,7 +1824,7 @@
         <v>10</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="K42" s="23" t="s">
         <v>10</v>
@@ -1871,19 +1832,19 @@
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D43" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G43" s="7">
         <v>0</v>
@@ -1893,39 +1854,39 @@
         <v>10</v>
       </c>
       <c r="J43" s="19" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="K43" s="23" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C44" s="7">
         <v>2</v>
       </c>
       <c r="D44" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G44" s="7">
         <v>0</v>
       </c>
       <c r="H44" s="33" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="K44" s="10" t="s">
         <v>10</v>
@@ -1933,10 +1894,10 @@
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C45" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="13">
         <v>0</v>
@@ -1945,16 +1906,16 @@
         <v>8</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="G45" s="13">
         <v>0</v>
       </c>
       <c r="H45" s="34" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>10</v>
@@ -1977,7 +1938,7 @@
     </row>
     <row r="47" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B47" s="1" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>1</v>
@@ -2021,25 +1982,19 @@
         <v>1</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G48" s="7">
         <v>5</v>
       </c>
       <c r="H48" s="7"/>
-      <c r="I48" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J48" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="K48" s="23" t="s">
-        <v>37</v>
-      </c>
+      <c r="I48" s="8"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="23"/>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B49" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>8</v>
@@ -2057,49 +2012,37 @@
         <v>4</v>
       </c>
       <c r="H49" s="7"/>
-      <c r="I49" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J49" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="K49" s="23" t="s">
-        <v>10</v>
-      </c>
+      <c r="I49" s="8"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="23"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B50" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="7">
+        <v>0</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="7">
-        <v>0</v>
-      </c>
-      <c r="E50" s="7">
-        <v>0</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G50" s="7">
         <v>4</v>
       </c>
       <c r="H50" s="7"/>
-      <c r="I50" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J50" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="K50" s="23" t="s">
-        <v>10</v>
-      </c>
+      <c r="I50" s="8"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="23"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B51" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C51" s="7">
         <v>1</v>
@@ -2111,27 +2054,21 @@
         <v>8</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G51" s="7">
         <v>0</v>
       </c>
       <c r="H51" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="I51" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J51" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="K51" s="10" t="s">
-        <v>10</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="I51" s="8"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="10"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B52" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C52" s="13">
         <v>1</v>
@@ -2143,23 +2080,17 @@
         <v>8</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="G52" s="13">
         <v>0</v>
       </c>
       <c r="H52" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="I52" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J52" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="K52" s="16" t="s">
-        <v>10</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I52" s="14"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="16"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B53" s="17"/>
@@ -2175,7 +2106,7 @@
     </row>
     <row r="54" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>1</v>
@@ -2213,13 +2144,13 @@
         <v>8</v>
       </c>
       <c r="D55" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G55" s="7">
         <v>2</v>
@@ -2229,27 +2160,27 @@
         <v>10</v>
       </c>
       <c r="J55" s="9" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="K55" s="23" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B56" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D56" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E56" s="7">
         <v>0</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G56" s="7">
         <v>3</v>
@@ -2259,7 +2190,7 @@
         <v>10</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="K56" s="23" t="s">
         <v>10</v>
@@ -2267,19 +2198,19 @@
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D57" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E57" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G57" s="7">
         <v>0</v>
@@ -2289,39 +2220,39 @@
         <v>10</v>
       </c>
       <c r="J57" s="19" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="K57" s="23" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B58" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C58" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D58" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>8</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G58" s="7">
         <v>0</v>
       </c>
       <c r="H58" s="33" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J58" s="9" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="K58" s="10" t="s">
         <v>10</v>
@@ -2329,7 +2260,7 @@
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C59" s="13">
         <v>0</v>
@@ -2341,13 +2272,13 @@
         <v>8</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="G59" s="13">
         <v>0</v>
       </c>
       <c r="H59" s="34" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="I59" s="14" t="s">
         <v>10</v>
@@ -2373,7 +2304,7 @@
     </row>
     <row r="61" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B61" s="1" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>1</v>
@@ -2411,13 +2342,13 @@
         <v>8</v>
       </c>
       <c r="D62" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E62" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G62" s="7">
         <v>3</v>
@@ -2427,15 +2358,15 @@
         <v>10</v>
       </c>
       <c r="J62" s="9" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="K62" s="23" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B63" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>8</v>
@@ -2444,10 +2375,10 @@
         <v>3</v>
       </c>
       <c r="E63" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G63" s="7">
         <v>2</v>
@@ -2457,15 +2388,15 @@
         <v>10</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="K63" s="23" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B64" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>8</v>
@@ -2477,7 +2408,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G64" s="7">
         <v>0</v>
@@ -2495,10 +2426,10 @@
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B65" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C65" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D65" s="7">
         <v>5</v>
@@ -2507,19 +2438,19 @@
         <v>8</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G65" s="7">
         <v>0</v>
       </c>
       <c r="H65" s="33" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="K65" s="10" t="s">
         <v>10</v>
@@ -2527,10 +2458,10 @@
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B66" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C66" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D66" s="13">
         <v>0</v>
@@ -2539,16 +2470,16 @@
         <v>8</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="G66" s="13">
         <v>0</v>
       </c>
       <c r="H66" s="34" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="I66" s="14" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="J66" s="25" t="s">
         <v>10</v>
@@ -2571,5 +2502,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Event Details PNG
</commit_message>
<xml_diff>
--- a/Reports/FP-Details.xlsx
+++ b/Reports/FP-Details.xlsx
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" zoomScale="51" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,7 +753,7 @@
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="69.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>